<commit_message>
update graphAnalysis test case
</commit_message>
<xml_diff>
--- a/src/main/resources/data/queryById.xlsx
+++ b/src/main/resources/data/queryById.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="13120"/>
+    <workbookView windowWidth="28000" windowHeight="7280"/>
   </bookViews>
   <sheets>
     <sheet name="工作表 1" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
     <t>图分析视图-queryById-同账号非当前项目标签不能查询视图数据</t>
   </si>
   <si>
-    <t>{"projectId":1426,"graphId":2827}</t>
+    <t>{"projectId":1426,"graphId":2837}</t>
   </si>
   <si>
     <t>无权操作</t>
@@ -133,13 +133,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
@@ -151,13 +144,6 @@
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -183,16 +169,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,15 +201,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -230,9 +238,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,14 +254,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,22 +282,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -316,175 +316,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,15 +576,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -601,16 +592,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -641,6 +632,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -657,16 +657,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -675,148 +675,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2035,7 +2035,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3303571428571" defaultRowHeight="19.9" customHeight="1" outlineLevelCol="5"/>

</xml_diff>